<commit_message>
Add script to sync public Excel
</commit_message>
<xml_diff>
--- a/data/bitacora.xlsx
+++ b/data/bitacora.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupokaufmann-my.sharepoint.com/personal/samuel_sanchez_grupokaufmann_com/Documents/Documentos/Dev/bitacora_diaria/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{4616FF0F-C10E-4DFE-8F27-869B9C60E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0512258D-D438-4C08-81B9-D22ABD3D194E}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{4616FF0F-C10E-4DFE-8F27-869B9C60E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00542452-2053-4315-9C1E-AA4CBA39ACA0}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15720" xr2:uid="{A9E3F017-9040-47A2-B586-0486128F3261}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$127</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="293">
   <si>
     <t>FLOTA</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>KKTT14</t>
+  </si>
+  <si>
+    <t>De Baja (Vendida)</t>
   </si>
   <si>
     <t>WDB932315K0250048</t>
@@ -922,7 +925,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1469,25 +1472,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA66EBA-6B88-4C75-8217-0B7E221D898D}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="11.453125" style="6"/>
+    <col min="1" max="1" width="39.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1539,7 +1542,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1562,7 +1565,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1585,7 +1588,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1608,7 +1611,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1634,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1654,7 +1657,7 @@
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1677,7 +1680,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1700,7 +1703,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1723,7 +1726,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1746,7 +1749,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -1770,7 +1773,7 @@
       <c r="I12" s="12"/>
       <c r="L12" s="26"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -1793,7 +1796,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -1816,7 +1819,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
@@ -1862,7 +1865,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1885,7 +1888,7 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -1908,7 +1911,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
@@ -1931,7 +1934,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="7" t="s">
         <v>50</v>
       </c>
@@ -1954,7 +1957,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>50</v>
       </c>
@@ -1977,7 +1980,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="7" t="s">
         <v>50</v>
       </c>
@@ -2000,7 +2003,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -2023,7 +2026,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="7" t="s">
         <v>58</v>
       </c>
@@ -2046,7 +2049,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="7" t="s">
         <v>64</v>
       </c>
@@ -2069,7 +2072,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="7" t="s">
         <v>64</v>
       </c>
@@ -2086,21 +2089,21 @@
         <v>53</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" s="9">
         <v>46112</v>
@@ -2109,21 +2112,21 @@
         <v>53</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D28" s="9">
         <v>46081</v>
@@ -2138,15 +2141,15 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29" s="9">
         <v>46053</v>
@@ -2161,15 +2164,15 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D30" s="9">
         <v>46204</v>
@@ -2184,15 +2187,15 @@
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D31" s="9">
         <v>46204</v>
@@ -2207,15 +2210,15 @@
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D32" s="9">
         <v>46204</v>
@@ -2230,15 +2233,15 @@
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" s="9">
         <v>46204</v>
@@ -2253,15 +2256,15 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D34" s="9">
         <v>46204</v>
@@ -2276,15 +2279,15 @@
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" s="9">
         <v>46204</v>
@@ -2299,15 +2302,15 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D36" s="9">
         <v>46204</v>
@@ -2322,50 +2325,50 @@
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D37" s="9">
         <v>46234</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G37" s="13">
         <v>46049</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D38" s="9">
         <v>46173</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>13</v>
@@ -2374,21 +2377,21 @@
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D39" s="9">
         <v>46173</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>13</v>
@@ -2397,21 +2400,21 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D40" s="9">
         <v>46173</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>13</v>
@@ -2420,21 +2423,21 @@
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D41" s="9">
         <v>46173</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>13</v>
@@ -2443,21 +2446,21 @@
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D42" s="9">
         <v>46173</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>13</v>
@@ -2466,21 +2469,21 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D43" s="9">
         <v>46173</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>13</v>
@@ -2489,21 +2492,21 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D44" s="9">
         <v>46173</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>13</v>
@@ -2512,21 +2515,21 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D45" s="9">
         <v>46173</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>13</v>
@@ -2535,79 +2538,79 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D46" s="9">
         <v>46173</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G46" s="13">
         <v>46042</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D47" s="9">
         <v>46173</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G47" s="13">
         <v>46043</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D48" s="9">
         <v>46173</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>13</v>
@@ -2616,50 +2619,50 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D49" s="9">
         <v>46234</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G49" s="13">
         <v>46049</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D50" s="9">
         <v>46234</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>13</v>
@@ -2668,21 +2671,21 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D51" s="9">
         <v>46234</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>13</v>
@@ -2691,21 +2694,21 @@
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D52" s="9">
         <v>46234</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>13</v>
@@ -2714,21 +2717,21 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D53" s="9">
         <v>46234</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>13</v>
@@ -2737,21 +2740,21 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D54" s="9">
         <v>46234</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>13</v>
@@ -2760,79 +2763,79 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D55" s="9">
         <v>46234</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G55" s="13">
         <v>46049</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D56" s="9">
         <v>46234</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G56" s="13">
         <v>46049</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D57" s="9">
         <v>46234</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>13</v>
@@ -2841,21 +2844,21 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D58" s="9">
         <v>46234</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>13</v>
@@ -2864,21 +2867,21 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D59" s="9">
         <v>46234</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>13</v>
@@ -2887,21 +2890,21 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9">
       <c r="A60" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D60" s="9">
         <v>46081</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>13</v>
@@ -2910,21 +2913,21 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9">
       <c r="A61" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D61" s="9">
         <v>46081</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>13</v>
@@ -2933,15 +2936,15 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9">
       <c r="A62" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D62" s="9">
         <v>46387</v>
@@ -2956,15 +2959,15 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9">
       <c r="A63" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D63" s="9">
         <v>46387</v>
@@ -2979,15 +2982,15 @@
       <c r="H63" s="12"/>
       <c r="I63" s="12"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9">
       <c r="A64" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D64" s="9">
         <v>46387</v>
@@ -3002,15 +3005,15 @@
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D65" s="9">
         <v>46387</v>
@@ -3025,15 +3028,15 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D66" s="9">
         <v>46387</v>
@@ -3048,15 +3051,15 @@
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9">
       <c r="A67" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D67" s="9">
         <v>46387</v>
@@ -3071,15 +3074,15 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9">
       <c r="A68" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D68" s="9">
         <v>46387</v>
@@ -3094,15 +3097,15 @@
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9">
       <c r="A69" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D69" s="9">
         <v>46387</v>
@@ -3117,15 +3120,15 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9">
       <c r="A70" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D70" s="9">
         <v>46387</v>
@@ -3140,15 +3143,15 @@
       <c r="H70" s="12"/>
       <c r="I70" s="12"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="A71" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D71" s="9">
         <v>46387</v>
@@ -3163,15 +3166,15 @@
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="A72" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D72" s="9">
         <v>46387</v>
@@ -3186,15 +3189,15 @@
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9">
       <c r="A73" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D73" s="9">
         <v>46053</v>
@@ -3209,15 +3212,15 @@
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="A74" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D74" s="9">
         <v>46053</v>
@@ -3232,15 +3235,15 @@
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="A75" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D75" s="9">
         <v>46081</v>
@@ -3255,15 +3258,15 @@
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="A76" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D76" s="9">
         <v>46081</v>
@@ -3278,15 +3281,15 @@
       <c r="H76" s="12"/>
       <c r="I76" s="12"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9">
       <c r="A77" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D77" s="9">
         <v>45991</v>
@@ -3301,15 +3304,15 @@
       <c r="H77" s="12"/>
       <c r="I77" s="12"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9">
       <c r="A78" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D78" s="9">
         <v>46081</v>
@@ -3324,15 +3327,15 @@
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9">
       <c r="A79" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D79" s="9">
         <v>45991</v>
@@ -3347,15 +3350,15 @@
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="A80" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D80" s="9">
         <v>45991</v>
@@ -3370,15 +3373,15 @@
       <c r="H80" s="12"/>
       <c r="I80" s="12"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9">
       <c r="A81" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D81" s="9">
         <v>46234</v>
@@ -3393,15 +3396,15 @@
       <c r="H81" s="12"/>
       <c r="I81" s="12"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9">
       <c r="A82" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D82" s="9">
         <v>46234</v>
@@ -3416,15 +3419,15 @@
       <c r="H82" s="12"/>
       <c r="I82" s="12"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9">
       <c r="A83" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D83" s="9">
         <v>46234</v>
@@ -3439,15 +3442,15 @@
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9">
       <c r="A84" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D84" s="9">
         <v>46081</v>
@@ -3462,15 +3465,15 @@
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9">
       <c r="A85" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D85" s="9">
         <v>45991</v>
@@ -3485,15 +3488,15 @@
       <c r="H85" s="12"/>
       <c r="I85" s="12"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9">
       <c r="A86" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D86" s="9">
         <v>45991</v>
@@ -3508,15 +3511,15 @@
       <c r="H86" s="12"/>
       <c r="I86" s="12"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9">
       <c r="A87" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D87" s="9">
         <v>46081</v>
@@ -3531,15 +3534,15 @@
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9">
       <c r="A88" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D88" s="9">
         <v>45991</v>
@@ -3554,15 +3557,15 @@
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9">
       <c r="A89" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D89" s="9">
         <v>45991</v>
@@ -3577,15 +3580,15 @@
       <c r="H89" s="12"/>
       <c r="I89" s="12"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9">
       <c r="A90" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D90" s="9">
         <v>45991</v>
@@ -3600,15 +3603,15 @@
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9">
       <c r="A91" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D91" s="9">
         <v>45658</v>
@@ -3623,15 +3626,15 @@
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9">
       <c r="A92" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D92" s="9">
         <v>45658</v>
@@ -3646,15 +3649,15 @@
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9">
       <c r="A93" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D93" s="9">
         <v>45658</v>
@@ -3669,50 +3672,50 @@
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9">
       <c r="A94" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D94" s="9">
         <v>46081</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G94" s="13">
         <v>46044</v>
       </c>
       <c r="H94" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I94" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D95" s="9">
         <v>46081</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>13</v>
@@ -3721,21 +3724,21 @@
       <c r="H95" s="12"/>
       <c r="I95" s="12"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9">
       <c r="A96" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D96" s="9">
         <v>46081</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F96" s="10" t="s">
         <v>13</v>
@@ -3744,12 +3747,12 @@
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9">
       <c r="A97" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C97" s="8">
         <v>65153</v>
@@ -3758,7 +3761,7 @@
         <v>47361</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>13</v>
@@ -3767,21 +3770,21 @@
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9">
       <c r="A98" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D98" s="9">
         <v>46356</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>13</v>
@@ -3790,21 +3793,21 @@
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9">
       <c r="A99" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D99" s="9">
         <v>46356</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F99" s="10" t="s">
         <v>13</v>
@@ -3813,21 +3816,21 @@
       <c r="H99" s="12"/>
       <c r="I99" s="12"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9">
       <c r="A100" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D100" s="9">
         <v>46053</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F100" s="10" t="s">
         <v>13</v>
@@ -3836,21 +3839,21 @@
       <c r="H100" s="12"/>
       <c r="I100" s="12"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9">
       <c r="A101" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D101" s="9">
         <v>46053</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F101" s="10" t="s">
         <v>13</v>
@@ -3859,429 +3862,429 @@
       <c r="H101" s="12"/>
       <c r="I101" s="12"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9">
       <c r="A102" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D102" s="9">
         <v>46996</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="12"/>
       <c r="I102" s="12"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9">
       <c r="A103" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D103" s="9">
         <v>46996</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G103" s="11"/>
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9">
       <c r="A104" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D104" s="9">
         <v>46996</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9">
       <c r="A105" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D105" s="9">
         <v>46996</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F105" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G105" s="11"/>
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9">
       <c r="A106" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D106" s="9">
         <v>46996</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G106" s="11"/>
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9">
       <c r="A107" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D107" s="9">
         <v>46996</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G107" s="11"/>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9">
       <c r="A108" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D108" s="9">
         <v>46996</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9">
       <c r="A109" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D109" s="9">
         <v>46996</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G109" s="11"/>
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9">
       <c r="A110" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D110" s="9">
         <v>46996</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9">
       <c r="A111" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D111" s="9">
         <v>46996</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9">
       <c r="A112" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D112" s="9">
         <v>46996</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G112" s="11"/>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9">
       <c r="A113" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D113" s="9">
         <v>46996</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G113" s="11"/>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9">
       <c r="A114" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D114" s="9">
         <v>46996</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G114" s="11"/>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9">
       <c r="A115" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D115" s="9">
         <v>46996</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F115" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G115" s="11"/>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9">
       <c r="A116" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D116" s="9">
         <v>46996</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F116" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G116" s="11"/>
       <c r="H116" s="12"/>
       <c r="I116" s="12"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9">
       <c r="A117" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D117" s="9">
         <v>46996</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G117" s="11"/>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9">
       <c r="A118" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D118" s="9">
         <v>46996</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F118" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G118" s="11"/>
       <c r="H118" s="12"/>
       <c r="I118" s="12"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9">
       <c r="A119" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D119" s="9">
         <v>46996</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G119" s="11"/>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9">
       <c r="A120" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D120" s="9">
         <v>45961</v>
@@ -4296,15 +4299,15 @@
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9">
       <c r="A121" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D121" s="9">
         <v>45961</v>
@@ -4319,15 +4322,15 @@
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9">
       <c r="A122" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D122" s="9">
         <v>45961</v>
@@ -4342,21 +4345,21 @@
       <c r="H122" s="12"/>
       <c r="I122" s="12"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9">
       <c r="A123" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D123" s="9">
         <v>46081</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F123" s="10" t="s">
         <v>13</v>
@@ -4365,15 +4368,15 @@
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9">
       <c r="A124" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D124" s="9">
         <v>46507</v>
@@ -4388,15 +4391,15 @@
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9">
       <c r="A125" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D125" s="9">
         <v>46507</v>
@@ -4411,15 +4414,15 @@
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9">
       <c r="A126" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D126" s="9">
         <v>46507</v>
@@ -4434,15 +4437,15 @@
       <c r="H126" s="12"/>
       <c r="I126" s="12"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9">
       <c r="A127" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D127" s="9">
         <v>46203</v>
@@ -4457,8 +4460,8 @@
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35"/>
-    <row r="129" x14ac:dyDescent="0.35"/>
+    <row r="128" spans="1:9"/>
+    <row r="129"/>
   </sheetData>
   <autoFilter ref="A1:F127" xr:uid="{EDA66EBA-6B88-4C75-8217-0B7E221D898D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4473,413 +4476,413 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="54" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:14">
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:14">
       <c r="D3" s="1">
         <v>868589060374017</v>
       </c>
       <c r="F3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G3" s="2" t="e">
         <f ca="1">VLOOKUP(D3,Hoja2!G:K,5,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" s="4">
         <v>46043</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:14">
       <c r="D4" s="1">
         <v>868589060674226</v>
       </c>
       <c r="F4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G4" s="2" t="e">
         <f ca="1">VLOOKUP(D4,Hoja2!G:K,5,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I4" s="4">
         <v>46043</v>
       </c>
     </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:14">
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:14">
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:14">
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:14">
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:14">
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:14">
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:14">
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:14">
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:14">
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:14">
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:14">
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:14">
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="13:14">
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="13:14">
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="13:14">
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="13:14">
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="13:14">
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="13:14">
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="13:14">
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="13:14">
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="13:14">
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="13:14">
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="13:14">
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="13:14">
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="13:14">
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="13:14">
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="13:14">
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="13:14">
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="13:14">
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="13:14">
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="13:14">
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:14">
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="13:14">
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="13:14">
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="13:14">
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="13:14">
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="13:14">
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="13:14">
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="13:14">
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="13:14">
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="13:14">
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="13:14">
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
     </row>
-    <row r="47" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="13:14">
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="13:14">
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="13:14">
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="13:14">
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="13:14">
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="13:14">
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="13:14">
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="13:14">
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="13:14">
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="13:14">
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="13:14">
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="13:14">
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="13:14">
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
     </row>
-    <row r="60" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="13:14">
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="13:14">
       <c r="M61" s="5"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="13:14">
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="13:14">
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="13:14">
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="13:14">
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="13:14">
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
     </row>
-    <row r="67" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="13:14">
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
     </row>
-    <row r="68" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="13:14">
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
     </row>
-    <row r="69" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="13:14">
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
     </row>
-    <row r="70" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="13:14">
       <c r="M70" s="5"/>
       <c r="N70" s="5"/>
     </row>
-    <row r="71" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="13:14">
       <c r="M71" s="5"/>
       <c r="N71" s="5"/>
     </row>
-    <row r="72" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="13:14">
       <c r="M72" s="5"/>
       <c r="N72" s="5"/>
     </row>
-    <row r="73" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="13:14">
       <c r="M73" s="5"/>
       <c r="N73" s="5"/>
     </row>
-    <row r="74" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="13:14">
       <c r="M74" s="5"/>
       <c r="N74" s="5"/>
     </row>
-    <row r="75" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="13:14">
       <c r="M75" s="5"/>
       <c r="N75" s="5"/>
     </row>
-    <row r="76" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="13:14">
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
     </row>
-    <row r="77" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="13:14">
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
     </row>
-    <row r="78" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="13:14">
       <c r="M78" s="5"/>
       <c r="N78" s="5"/>
     </row>
-    <row r="79" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="13:14">
       <c r="M79" s="5"/>
       <c r="N79" s="5"/>
     </row>
-    <row r="80" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="13:14">
       <c r="M80" s="5"/>
       <c r="N80" s="5"/>
     </row>
-    <row r="81" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="13:14">
       <c r="M81" s="5"/>
       <c r="N81" s="5"/>
     </row>
-    <row r="82" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="13:14">
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
     </row>
-    <row r="83" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="13:14">
       <c r="M83" s="5"/>
       <c r="N83" s="5"/>
     </row>
-    <row r="84" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="13:14">
       <c r="M84" s="5"/>
       <c r="N84" s="5"/>
     </row>
-    <row r="85" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="13:14">
       <c r="M85" s="5"/>
       <c r="N85" s="5"/>
     </row>
-    <row r="86" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="13:14">
       <c r="M86" s="5"/>
       <c r="N86" s="5"/>
     </row>
-    <row r="87" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="13:14">
       <c r="M87" s="5"/>
       <c r="N87" s="5"/>
     </row>
-    <row r="88" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="13:14">
       <c r="M88" s="5"/>
       <c r="N88" s="5"/>
     </row>
-    <row r="89" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="13:14">
       <c r="M89" s="5"/>
       <c r="N89" s="5"/>
     </row>
-    <row r="90" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="13:14">
       <c r="M90" s="5"/>
       <c r="N90" s="5"/>
     </row>
-    <row r="91" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="13:14">
       <c r="M91" s="5"/>
       <c r="N91" s="5"/>
     </row>
-    <row r="92" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="13:14">
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
     </row>
@@ -4889,6 +4892,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100027709BF533FA442AFC4A8B2C0110727" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a37fc0d7c302f7619d355a49e1f175a4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a" xmlns:ns4="bda9c1ec-c4e2-44f9-929c-ca399fe36c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01250a30c504a808427f15ccf149ee4d" ns3:_="" ns4:_="">
     <xsd:import namespace="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a"/>
@@ -5121,56 +5141,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4794C7E6-B89D-4081-9A67-B8D500EF1EE4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a"/>
-    <ds:schemaRef ds:uri="bda9c1ec-c4e2-44f9-929c-ca399fe36c88"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9861A25-610F-425F-BC6A-AC52D4971411}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C8123E5-81FD-4C24-91F1-33BC079967E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C8123E5-81FD-4C24-91F1-33BC079967E9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9861A25-610F-425F-BC6A-AC52D4971411}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e53c16e-6636-411e-b1c4-e9eeb71b3b2a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4794C7E6-B89D-4081-9A67-B8D500EF1EE4}"/>
 </file>
</xml_diff>

<commit_message>
chore: daily sync bitacora
</commit_message>
<xml_diff>
--- a/data/bitacora.xlsx
+++ b/data/bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupokaufmann-my.sharepoint.com/personal/samuel_sanchez_grupokaufmann_com/Documents/Documentos/Dev/bitacora_diaria/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{4616FF0F-C10E-4DFE-8F27-869B9C60E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00542452-2053-4315-9C1E-AA4CBA39ACA0}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{4616FF0F-C10E-4DFE-8F27-869B9C60E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7C8B8C5-D872-43BF-AE5D-CE340017A35B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15720" xr2:uid="{A9E3F017-9040-47A2-B586-0486128F3261}"/>
   </bookViews>
@@ -249,7 +249,7 @@
     <t>KKTT14</t>
   </si>
   <si>
-    <t>De Baja (Vendida)</t>
+    <t xml:space="preserve">De Baja </t>
   </si>
   <si>
     <t>WDB932315K0250048</t>
@@ -1472,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA66EBA-6B88-4C75-8217-0B7E221D898D}">
   <dimension ref="A1:L129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>